<commit_message>
Added sample jxls query with multiple worksheets to demo database Modified admin jsp pages to use user/footer.jsp
</commit_message>
<xml_diff>
--- a/art/src/art/WEB-INF/templates/sample-jxls1.xlsx
+++ b/art/src/art/WEB-INF/templates/sample-jxls1.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Sample jxls report</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Volume</t>
+  </si>
+  <si>
+    <t>$[SUM(E11)]</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
@@ -77,7 +83,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -157,7 +163,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,6 +555,14 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>